<commit_message>
Global Irminger - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GI03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GI03FLMA_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1180" windowWidth="24780" windowHeight="12960" activeTab="1"/>
+    <workbookView xWindow="1360" yWindow="1180" windowWidth="24780" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1601,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="8">
-        <v>41955</v>
+        <v>41894</v>
       </c>
       <c r="F2" s="13">
         <v>0.84097222222222223</v>
@@ -1651,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>